<commit_message>
Automatische test-sync: 2025-06-25 22:43:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-25.xlsx
+++ b/logs/mail_log_2025-06-25.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -732,24 +732,59 @@
           <t>Factuur / Administratie</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>2025-06-25 22:40:03</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-06-25 22:43:26</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>Ja</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -769,7 +804,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -787,7 +822,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -817,6 +852,16 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-25 22:44:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-25.xlsx
+++ b/logs/mail_log_2025-06-25.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -783,8 +783,45 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Verzoek om factuur</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Testmail #1: Verzoek om factuur</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-06-25 22:44:14</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -804,7 +841,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -849,7 +886,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>